<commit_message>
tgc prototype: 1 inch chits!! /play yeah
</commit_message>
<xml_diff>
--- a/data/security_tokens.xlsx
+++ b/data/security_tokens.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="6645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="6645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Security Tokens" sheetId="1" r:id="rId1"/>
+    <sheet name="Large Circle Chits" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -102,6 +103,150 @@
   </si>
   <si>
     <t>File</t>
+  </si>
+  <si>
+    <t>Img</t>
+  </si>
+  <si>
+    <t>reinforcements.svg</t>
+  </si>
+  <si>
+    <t>#42290d</t>
+  </si>
+  <si>
+    <t>reinforcements</t>
+  </si>
+  <si>
+    <t>asterisk</t>
+  </si>
+  <si>
+    <t>records</t>
+  </si>
+  <si>
+    <t>asterisk.svg</t>
+  </si>
+  <si>
+    <t>control_panel.svg</t>
+  </si>
+  <si>
+    <t>control_panel_cyan</t>
+  </si>
+  <si>
+    <t>control_panel_purple</t>
+  </si>
+  <si>
+    <t>control_panel_yellow</t>
+  </si>
+  <si>
+    <t>#40bfbd</t>
+  </si>
+  <si>
+    <t>#bf40ba</t>
+  </si>
+  <si>
+    <t>BGColor</t>
+  </si>
+  <si>
+    <t>FGColor</t>
+  </si>
+  <si>
+    <t>#d8c586</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
+  <si>
+    <t>records.svg</t>
+  </si>
+  <si>
+    <t>#bbd329</t>
+  </si>
+  <si>
+    <t>entrance</t>
+  </si>
+  <si>
+    <t>entrance.svg</t>
+  </si>
+  <si>
+    <t>Overlay</t>
+  </si>
+  <si>
+    <t>linen.png</t>
+  </si>
+  <si>
+    <t>art_apple</t>
+  </si>
+  <si>
+    <t>art_fakeapple</t>
+  </si>
+  <si>
+    <t>art_apple.svg</t>
+  </si>
+  <si>
+    <t>art_fakeapple.svg</t>
+  </si>
+  <si>
+    <t>#d8c587</t>
+  </si>
+  <si>
+    <t>art_strawberry</t>
+  </si>
+  <si>
+    <t>art_strawberry.svg</t>
+  </si>
+  <si>
+    <t>art_fakestrawberry</t>
+  </si>
+  <si>
+    <t>art_fakestrawberry.svg</t>
+  </si>
+  <si>
+    <t>art_grapes</t>
+  </si>
+  <si>
+    <t>art_fakegrapes</t>
+  </si>
+  <si>
+    <t>art_fakegrapes.svg</t>
+  </si>
+  <si>
+    <t>art_grapes.svg</t>
+  </si>
+  <si>
+    <t>art_house</t>
+  </si>
+  <si>
+    <t>art_house.svg</t>
+  </si>
+  <si>
+    <t>art_fakehouse</t>
+  </si>
+  <si>
+    <t>art_fakehouse.svg</t>
+  </si>
+  <si>
+    <t>art_church</t>
+  </si>
+  <si>
+    <t>art_fakechurch</t>
+  </si>
+  <si>
+    <t>art_church.svg</t>
+  </si>
+  <si>
+    <t>art_fakechurch.svg</t>
+  </si>
+  <si>
+    <t>art_lighthouse</t>
+  </si>
+  <si>
+    <t>art_lighthouse.svg</t>
+  </si>
+  <si>
+    <t>art_fakelighthouse</t>
+  </si>
+  <si>
+    <t>art_fakelighthouse.svg</t>
   </si>
 </sst>
 </file>
@@ -145,9 +290,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,7 +581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -636,4 +787,489 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="3">
+        <v>2</v>
+      </c>
+      <c r="G2" t="str">
+        <f>"circle_"&amp;A2&amp;"[all,"&amp;F2&amp;"]"</f>
+        <v>circle_reinforcements[all,2]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="str">
+        <f>"circle_"&amp;A3&amp;"[all,"&amp;F3&amp;"]"</f>
+        <v>circle_asterisk[all,1]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" t="str">
+        <f>"circle_"&amp;A4&amp;"[all,"&amp;F4&amp;"]"</f>
+        <v>circle_control_panel_cyan[all,1]</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" t="str">
+        <f>"circle_"&amp;A5&amp;"[all,"&amp;F5&amp;"]"</f>
+        <v>circle_control_panel_purple[all,1]</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" t="str">
+        <f>"circle_"&amp;A6&amp;"[all,"&amp;F6&amp;"]"</f>
+        <v>circle_control_panel_yellow[all,1]</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+      <c r="G7" t="str">
+        <f>"circle_"&amp;A7&amp;"[all,"&amp;F7&amp;"]"</f>
+        <v>circle_records[all,2]</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="3">
+        <v>4</v>
+      </c>
+      <c r="G8" t="str">
+        <f>"square_"&amp;A8&amp;"[all,"&amp;F8&amp;"]"</f>
+        <v>square_entrance[all,4]</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" t="str">
+        <f>"square_"&amp;A9&amp;"[all,"&amp;F9&amp;"]"</f>
+        <v>square_art_apple[all,1]</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" t="str">
+        <f>"square_"&amp;A10&amp;"[all,"&amp;F10&amp;"]"</f>
+        <v>square_art_fakeapple[all,1]</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" t="str">
+        <f>"square_"&amp;A11&amp;"[all,"&amp;F11&amp;"]"</f>
+        <v>square_art_strawberry[all,1]</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" t="str">
+        <f>"square_"&amp;A12&amp;"[all,"&amp;F12&amp;"]"</f>
+        <v>square_art_fakestrawberry[all,1]</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" ref="G13:G20" si="0">"square_"&amp;A13&amp;"[all,"&amp;F13&amp;"]"</f>
+        <v>square_art_grapes[all,1]</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>square_art_fakegrapes[all,1]</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>square_art_house[all,1]</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>square_art_fakehouse[all,1]</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>square_art_church[all,1]</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>square_art_fakechurch[all,1]</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>square_art_lighthouse[all,1]</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>square_art_fakelighthouse[all,1]</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tgc prototype: small chits!
</commit_message>
<xml_diff>
--- a/data/security_tokens.xlsx
+++ b/data/security_tokens.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="6645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="6645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Security Tokens" sheetId="1" r:id="rId1"/>
-    <sheet name="Large Circle Chits" sheetId="2" r:id="rId2"/>
+    <sheet name="Large Chits" sheetId="2" r:id="rId2"/>
+    <sheet name="Small Chits" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="87">
   <si>
     <t>Name</t>
   </si>
@@ -247,6 +248,45 @@
   </si>
   <si>
     <t>art_fakelighthouse.svg</t>
+  </si>
+  <si>
+    <t>ideas</t>
+  </si>
+  <si>
+    <t>idea.svg</t>
+  </si>
+  <si>
+    <t>plan_blue</t>
+  </si>
+  <si>
+    <t>plan_red</t>
+  </si>
+  <si>
+    <t>plan_green</t>
+  </si>
+  <si>
+    <t>plan_black</t>
+  </si>
+  <si>
+    <t>plan.svg</t>
+  </si>
+  <si>
+    <t>#d8c588</t>
+  </si>
+  <si>
+    <t>#d8c589</t>
+  </si>
+  <si>
+    <t>#d8c590</t>
+  </si>
+  <si>
+    <t>#008630</t>
+  </si>
+  <si>
+    <t>#073bb2</t>
+  </si>
+  <si>
+    <t>#dc160c</t>
   </si>
 </sst>
 </file>
@@ -793,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,4 +1312,192 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="3">
+        <v>36</v>
+      </c>
+      <c r="G2" t="str">
+        <f>"circle_"&amp;A2&amp;"[all,"&amp;F2&amp;"]"</f>
+        <v>circle_ideas[all,36]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="3">
+        <v>12</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G6" si="0">"circle_"&amp;A3&amp;"[all,"&amp;F3&amp;"]"</f>
+        <v>circle_plan_blue[all,12]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="3">
+        <v>12</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>circle_plan_red[all,12]</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="3">
+        <v>12</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>circle_plan_green[all,12]</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="3">
+        <v>12</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>circle_plan_black[all,12]</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
chits: no more linen
</commit_message>
<xml_diff>
--- a/data/security_tokens.xlsx
+++ b/data/security_tokens.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="6645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="6645"/>
   </bookViews>
   <sheets>
     <sheet name="Security Tokens" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -167,12 +167,6 @@
   </si>
   <si>
     <t>entrance.svg</t>
-  </si>
-  <si>
-    <t>Overlay</t>
-  </si>
-  <si>
-    <t>linen.png</t>
   </si>
   <si>
     <t>art_apple</t>
@@ -621,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,10 +825,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G20"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,12 +836,11 @@
     <col min="1" max="1" width="17.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -860,17 +853,14 @@
       <c r="D1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -883,15 +873,15 @@
       <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="3">
+      <c r="E2" s="3">
         <v>2</v>
       </c>
-      <c r="G2" t="str">
-        <f>"circle_"&amp;A2&amp;"[all,"&amp;F2&amp;"]"</f>
+      <c r="F2" t="str">
+        <f>"circle_"&amp;A2&amp;"[all,"&amp;E2&amp;"]"</f>
         <v>circle_reinforcements[all,2]</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -904,15 +894,15 @@
       <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="str">
-        <f>"circle_"&amp;A3&amp;"[all,"&amp;F3&amp;"]"</f>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="str">
+        <f>"circle_"&amp;A3&amp;"[all,"&amp;E3&amp;"]"</f>
         <v>circle_asterisk[all,1]</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -925,15 +915,15 @@
       <c r="D4" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="3">
-        <v>1</v>
-      </c>
-      <c r="G4" t="str">
-        <f>"circle_"&amp;A4&amp;"[all,"&amp;F4&amp;"]"</f>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" t="str">
+        <f>"circle_"&amp;A4&amp;"[all,"&amp;E4&amp;"]"</f>
         <v>circle_control_panel_cyan[all,1]</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -946,15 +936,15 @@
       <c r="D5" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="3">
-        <v>1</v>
-      </c>
-      <c r="G5" t="str">
-        <f>"circle_"&amp;A5&amp;"[all,"&amp;F5&amp;"]"</f>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" t="str">
+        <f>"circle_"&amp;A5&amp;"[all,"&amp;E5&amp;"]"</f>
         <v>circle_control_panel_purple[all,1]</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -967,15 +957,15 @@
       <c r="D6" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="3">
-        <v>1</v>
-      </c>
-      <c r="G6" t="str">
-        <f>"circle_"&amp;A6&amp;"[all,"&amp;F6&amp;"]"</f>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" t="str">
+        <f>"circle_"&amp;A6&amp;"[all,"&amp;E6&amp;"]"</f>
         <v>circle_control_panel_yellow[all,1]</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -988,15 +978,15 @@
       <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="3">
+      <c r="E7" s="3">
         <v>2</v>
       </c>
-      <c r="G7" t="str">
-        <f>"circle_"&amp;A7&amp;"[all,"&amp;F7&amp;"]"</f>
+      <c r="F7" t="str">
+        <f>"circle_"&amp;A7&amp;"[all,"&amp;E7&amp;"]"</f>
         <v>circle_records[all,2]</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -1009,23 +999,20 @@
       <c r="D8" t="s">
         <v>41</v>
       </c>
-      <c r="E8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="3">
+      <c r="E8" s="3">
         <v>4</v>
       </c>
-      <c r="G8" t="str">
-        <f>"square_"&amp;A8&amp;"[all,"&amp;F8&amp;"]"</f>
+      <c r="F8" t="str">
+        <f>"square_"&amp;A8&amp;"[all,"&amp;E8&amp;"]"</f>
         <v>square_entrance[all,4]</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
         <v>49</v>
-      </c>
-      <c r="B9" t="s">
-        <v>51</v>
       </c>
       <c r="C9" t="s">
         <v>28</v>
@@ -1033,278 +1020,242 @@
       <c r="D9" t="s">
         <v>41</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" t="str">
+        <f>"square_"&amp;A9&amp;"[all,"&amp;E9&amp;"]"</f>
+        <v>square_art_apple[all,1]</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="3">
-        <v>1</v>
-      </c>
-      <c r="G9" t="str">
-        <f>"square_"&amp;A9&amp;"[all,"&amp;F9&amp;"]"</f>
-        <v>square_art_apple[all,1]</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>50</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" t="str">
+        <f>"square_"&amp;A10&amp;"[all,"&amp;E10&amp;"]"</f>
+        <v>square_art_fakeapple[all,1]</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>52</v>
       </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B11" t="s">
         <v>53</v>
       </c>
-      <c r="E10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="3">
-        <v>1</v>
-      </c>
-      <c r="G10" t="str">
-        <f>"square_"&amp;A10&amp;"[all,"&amp;F10&amp;"]"</f>
-        <v>square_art_fakeapple[all,1]</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" t="str">
+        <f>"square_"&amp;A11&amp;"[all,"&amp;E11&amp;"]"</f>
+        <v>square_art_strawberry[all,1]</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>54</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>55</v>
       </c>
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="3">
-        <v>1</v>
-      </c>
-      <c r="G11" t="str">
-        <f>"square_"&amp;A11&amp;"[all,"&amp;F11&amp;"]"</f>
-        <v>square_art_strawberry[all,1]</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" t="str">
+        <f>"square_"&amp;A12&amp;"[all,"&amp;E12&amp;"]"</f>
+        <v>square_art_fakestrawberry[all,1]</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>56</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" t="str">
+        <f>"square_"&amp;A13&amp;"[all,"&amp;E13&amp;"]"</f>
+        <v>square_art_grapes[all,1]</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>57</v>
       </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="3">
-        <v>1</v>
-      </c>
-      <c r="G12" t="str">
-        <f>"square_"&amp;A12&amp;"[all,"&amp;F12&amp;"]"</f>
-        <v>square_art_fakestrawberry[all,1]</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B14" t="s">
         <v>58</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" t="str">
+        <f>"square_"&amp;A14&amp;"[all,"&amp;E14&amp;"]"</f>
+        <v>square_art_fakegrapes[all,1]</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s">
         <v>61</v>
       </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="3">
-        <v>1</v>
-      </c>
-      <c r="G13" t="str">
-        <f t="shared" ref="G13:G20" si="0">"square_"&amp;A13&amp;"[all,"&amp;F13&amp;"]"</f>
-        <v>square_art_grapes[all,1]</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="3">
-        <v>1</v>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" si="0"/>
-        <v>square_art_fakegrapes[all,1]</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" t="str">
+        <f>"square_"&amp;A15&amp;"[all,"&amp;E15&amp;"]"</f>
+        <v>square_art_house[all,1]</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>62</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>63</v>
       </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="3">
-        <v>1</v>
-      </c>
-      <c r="G15" t="str">
-        <f t="shared" si="0"/>
-        <v>square_art_house[all,1]</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" t="str">
+        <f>"square_"&amp;A16&amp;"[all,"&amp;E16&amp;"]"</f>
+        <v>square_art_fakehouse[all,1]</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>64</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" t="str">
+        <f>"square_"&amp;A17&amp;"[all,"&amp;E17&amp;"]"</f>
+        <v>square_art_church[all,1]</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>65</v>
       </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="3">
-        <v>1</v>
-      </c>
-      <c r="G16" t="str">
-        <f t="shared" si="0"/>
-        <v>square_art_fakehouse[all,1]</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" t="str">
+        <f>"square_"&amp;A18&amp;"[all,"&amp;E18&amp;"]"</f>
+        <v>square_art_fakechurch[all,1]</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>68</v>
       </c>
-      <c r="C17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="3">
-        <v>1</v>
-      </c>
-      <c r="G17" t="str">
-        <f t="shared" si="0"/>
-        <v>square_art_church[all,1]</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>69</v>
       </c>
-      <c r="C18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="3">
-        <v>1</v>
-      </c>
-      <c r="G18" t="str">
-        <f t="shared" si="0"/>
-        <v>square_art_fakechurch[all,1]</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" t="str">
+        <f>"square_"&amp;A19&amp;"[all,"&amp;E19&amp;"]"</f>
+        <v>square_art_lighthouse[all,1]</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>70</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>71</v>
       </c>
-      <c r="C19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
-      <c r="G19" t="str">
-        <f t="shared" si="0"/>
-        <v>square_art_lighthouse[all,1]</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" t="s">
-        <v>73</v>
-      </c>
       <c r="C20" t="s">
         <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="3">
-        <v>1</v>
-      </c>
-      <c r="G20" t="str">
-        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" t="str">
+        <f>"square_"&amp;A20&amp;"[all,"&amp;E20&amp;"]"</f>
         <v>square_art_fakelighthouse[all,1]</v>
       </c>
     </row>
@@ -1316,15 +1267,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1337,22 +1288,19 @@
       <c r="D1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
@@ -1360,142 +1308,139 @@
       <c r="D2" t="s">
         <v>41</v>
       </c>
-      <c r="E2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="E2" s="3">
         <v>36</v>
       </c>
-      <c r="G2" t="str">
-        <f>"circle_"&amp;A2&amp;"[all,"&amp;F2&amp;"]"</f>
+      <c r="F2" t="str">
+        <f>"circle_"&amp;A2&amp;"[all,"&amp;E2&amp;"]"</f>
         <v>circle_ideas[all,36]</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="3">
+        <v>12</v>
+      </c>
+      <c r="F3" t="str">
+        <f>"circle_"&amp;A3&amp;"[all,"&amp;E3&amp;"]"</f>
+        <v>circle_plan_blue[all,12]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="3">
+        <v>12</v>
+      </c>
+      <c r="F4" t="str">
+        <f>"circle_"&amp;A4&amp;"[all,"&amp;E4&amp;"]"</f>
+        <v>circle_plan_red[all,12]</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>76</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
         <v>80</v>
       </c>
-      <c r="C3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="D5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="3">
         <v>12</v>
       </c>
-      <c r="G3" t="str">
-        <f t="shared" ref="G3:G6" si="0">"circle_"&amp;A3&amp;"[all,"&amp;F3&amp;"]"</f>
-        <v>circle_plan_blue[all,12]</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F5" t="str">
+        <f>"circle_"&amp;A5&amp;"[all,"&amp;E5&amp;"]"</f>
+        <v>circle_plan_green[all,12]</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>77</v>
       </c>
-      <c r="B4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
         <v>81</v>
-      </c>
-      <c r="D4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="3">
-        <v>12</v>
-      </c>
-      <c r="G4" t="str">
-        <f t="shared" si="0"/>
-        <v>circle_plan_red[all,12]</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" s="3">
-        <v>12</v>
-      </c>
-      <c r="G5" t="str">
-        <f t="shared" si="0"/>
-        <v>circle_plan_green[all,12]</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" t="s">
-        <v>83</v>
       </c>
       <c r="D6" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="3">
+      <c r="E6" s="3">
         <v>12</v>
       </c>
-      <c r="G6" t="str">
-        <f t="shared" si="0"/>
+      <c r="F6" t="str">
+        <f>"circle_"&amp;A6&amp;"[all,"&amp;E6&amp;"]"</f>
         <v>circle_plan_black[all,12]</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="3"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>